<commit_message>
Changed questions slightly and truncated the questions we will be asking
</commit_message>
<xml_diff>
--- a/eeg_data/meta_sheet.xlsx
+++ b/eeg_data/meta_sheet.xlsx
@@ -256,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +266,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,15 +315,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,53 +673,60 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="6"/>
       <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -727,18 +761,18 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -759,24 +793,28 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -827,70 +865,80 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="6" t="s">
         <v>53</v>
       </c>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">

</xml_diff>